<commit_message>
dodałem z trendsów wyniki do danych
</commit_message>
<xml_diff>
--- a/Data/data_combined.xlsx
+++ b/Data/data_combined.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">Patents_amount_on_companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vissystemsGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensorsGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aiGT</t>
   </si>
   <si>
     <t xml:space="preserve">2008</t>
@@ -94,7 +103,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -132,12 +141,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -189,7 +192,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,10 +206,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -226,7 +225,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,10 +247,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -259,15 +258,15 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -299,7 +298,7 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
@@ -308,23 +307,41 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="n">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="n">
         <v>9.9</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>22913</v>
       </c>
+      <c r="M2" s="0" t="n">
+        <v>340</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>507</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>582</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="n">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="n">
         <v>10.3</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -333,12 +350,21 @@
       <c r="K3" s="0" t="n">
         <v>22913</v>
       </c>
+      <c r="M3" s="0" t="n">
+        <v>279</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>487</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>639</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="n">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>11.1</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -350,12 +376,21 @@
       <c r="L4" s="0" t="n">
         <v>2209</v>
       </c>
+      <c r="M4" s="0" t="n">
+        <v>258</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>455</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>692</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="n">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <v>12.2</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -367,12 +402,21 @@
       <c r="L5" s="0" t="n">
         <v>2449</v>
       </c>
+      <c r="M5" s="0" t="n">
+        <v>225</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>419</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>599</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="n">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="n">
         <v>13.5</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -387,18 +431,27 @@
       <c r="L6" s="0" t="n">
         <v>2718</v>
       </c>
+      <c r="M6" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>407</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>677</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="n">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="n">
         <v>14.4</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>37088</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="6" t="n">
         <v>0.25</v>
       </c>
       <c r="J7" s="0" t="n">
@@ -410,12 +463,21 @@
       <c r="L7" s="0" t="n">
         <v>3186</v>
       </c>
+      <c r="M7" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>414</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>601</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="6" t="n">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="n">
         <v>15.7</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -427,7 +489,7 @@
       <c r="H8" s="0" t="n">
         <v>1.11</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="6" t="n">
         <v>0.43</v>
       </c>
       <c r="J8" s="0" t="n">
@@ -439,12 +501,21 @@
       <c r="L8" s="0" t="n">
         <v>3699</v>
       </c>
+      <c r="M8" s="0" t="n">
+        <v>153</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>432</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>659</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="5" t="n">
         <v>17.1</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -459,10 +530,10 @@
       <c r="G9" s="0" t="n">
         <v>5850</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="7" t="n">
         <v>1.23</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="6" t="n">
         <v>0.91</v>
       </c>
       <c r="J9" s="0" t="n">
@@ -474,12 +545,21 @@
       <c r="L9" s="0" t="n">
         <v>4406</v>
       </c>
+      <c r="M9" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>455</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>675</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="4" t="n">
         <v>2016</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="5" t="n">
         <v>18.7</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -494,10 +574,10 @@
       <c r="G10" s="0" t="n">
         <v>8660</v>
       </c>
-      <c r="H10" s="8" t="n">
+      <c r="H10" s="7" t="n">
         <v>1.32</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I10" s="6" t="n">
         <v>1.2</v>
       </c>
       <c r="J10" s="0" t="n">
@@ -509,12 +589,21 @@
       <c r="L10" s="0" t="n">
         <v>5471</v>
       </c>
+      <c r="M10" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>455</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>635</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="5" t="n">
         <v>20.3</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -529,10 +618,10 @@
       <c r="G11" s="0" t="n">
         <v>12560</v>
       </c>
-      <c r="H11" s="8" t="n">
+      <c r="H11" s="7" t="n">
         <v>1.45</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="6" t="n">
         <v>2.1</v>
       </c>
       <c r="J11" s="0" t="n">
@@ -544,10 +633,19 @@
       <c r="L11" s="0" t="n">
         <v>6873</v>
       </c>
+      <c r="M11" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>478</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>795</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>19</v>
+      <c r="A12" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>8.5</v>
@@ -564,10 +662,10 @@
       <c r="G12" s="0" t="n">
         <v>20000</v>
       </c>
-      <c r="H12" s="8" t="n">
+      <c r="H12" s="7" t="n">
         <v>1.56</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="6" t="n">
         <v>2.75</v>
       </c>
       <c r="J12" s="0" t="n">
@@ -579,10 +677,19 @@
       <c r="L12" s="0" t="n">
         <v>8948</v>
       </c>
+      <c r="M12" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>478</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>888</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>10.4</v>
@@ -596,10 +703,10 @@
       <c r="G13" s="0" t="n">
         <v>33510</v>
       </c>
-      <c r="H13" s="8" t="n">
+      <c r="H13" s="7" t="n">
         <v>1.68</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="6" t="n">
         <v>4.69</v>
       </c>
       <c r="J13" s="0" t="n">
@@ -610,6 +717,15 @@
       </c>
       <c r="L13" s="0" t="n">
         <v>9487</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>475</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>952</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +741,10 @@
       <c r="F14" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="H14" s="8" t="n">
+      <c r="H14" s="7" t="n">
         <v>1.8</v>
       </c>
-      <c r="I14" s="8"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">

</xml_diff>